<commit_message>
Excel Report Updation and Devtest Crediential Changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DEVTEST- IB Validation Report.xlsx
+++ b/src/test/resources/testdata/DEVTEST- IB Validation Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.udhaya.suriyan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.udhaya.suriyan\Automation_GIT\ART_TestAutomationCode_11\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65318B3-03B1-4E45-93BB-50C728719325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC727411-EBD6-4E55-9E2D-E30C7BE7D5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CC520112-56BE-497B-8AC8-7A27D633521F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="35">
   <si>
     <t>NA</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Story</t>
   </si>
   <si>
-    <t>Feature</t>
-  </si>
-  <si>
     <t>Epic</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Not Flown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature </t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,13 +569,13 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>24</v>
@@ -638,206 +638,197 @@
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>2</v>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>0</v>
+      <c r="R2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>2</v>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>0</v>
+      <c r="R3" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>0</v>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>0</v>
@@ -857,37 +848,37 @@
       <c r="O5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>0</v>
+      <c r="P5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
+      <c r="B6" t="s">
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>2</v>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>0</v>
@@ -922,66 +913,63 @@
       <c r="Q6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="R6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>0</v>
+      <c r="R6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S6" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>2</v>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" t="s">
+        <v>33</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>2</v>
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" t="s">
+        <v>33</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R7" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -989,39 +977,12 @@
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="K8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="M8" s="3" t="s">
         <v>0</v>
       </c>
@@ -1035,21 +996,15 @@
         <v>0</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S8" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -1059,13 +1014,13 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>14</v>
@@ -1076,25 +1031,10 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>